<commit_message>
BIS-1630: fixed import tests
</commit_message>
<xml_diff>
--- a/server-application-server/sourceTest/java/ch/ethz/sis/openbis/systemtest/asapi/v3/test_files/import/existing_vocabulary.xlsx
+++ b/server-application-server/sourceTest/java/ch/ethz/sis/openbis/systemtest/asapi/v3/test_files/import/existing_vocabulary.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="15">
   <si>
     <t xml:space="preserve">VOCABULARY_TYPE</t>
   </si>
@@ -31,10 +31,16 @@
     <t xml:space="preserve">Code</t>
   </si>
   <si>
+    <t xml:space="preserve">Internal</t>
+  </si>
+  <si>
     <t xml:space="preserve">Description</t>
   </si>
   <si>
     <t xml:space="preserve">TEST_VOCABULARY</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FALSE</t>
   </si>
   <si>
     <t xml:space="preserve">Test vocabulary with modifications</t>
@@ -184,17 +190,17 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D7"/>
+  <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C4" activeCellId="0" sqref="C4"/>
+      <selection pane="topLeft" activeCell="C9" activeCellId="0" sqref="C9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.39453125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.3984375" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="21"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="37"/>
@@ -217,41 +223,53 @@
       <c r="C2" s="1" t="s">
         <v>3</v>
       </c>
+      <c r="D2" s="1" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="2" t="n">
         <v>1</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="18.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>6</v>
+      </c>
+      <c r="D3" s="0" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="3" t="s">
         <v>1</v>
       </c>
       <c r="B4" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="C4" s="4" t="s">
+      <c r="C4" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="B5" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="C5" s="0" t="s">
         <v>6</v>
       </c>
-      <c r="D4" s="4" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="2" t="n">
-        <v>1</v>
-      </c>
-      <c r="B5" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="C5" s="0" t="s">
-        <v>8</v>
+      <c r="D5" s="0" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -259,10 +277,13 @@
         <v>1</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>10</v>
+        <v>6</v>
+      </c>
+      <c r="D6" s="0" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -270,12 +291,15 @@
         <v>1</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>12</v>
-      </c>
-      <c r="D7" s="4"/>
+        <v>6</v>
+      </c>
+      <c r="D7" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="E7" s="4"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>